<commit_message>
updated to include component strategy
</commit_message>
<xml_diff>
--- a/i_test/test_D3_bleeding_components/bleeding_narrow.xlsx
+++ b/i_test/test_D3_bleeding_components/bleeding_narrow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -55,6 +55,30 @@
   </si>
   <si>
     <t>hospital_main_diagnosis</t>
+  </si>
+  <si>
+    <t>pres</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>P04</t>
+  </si>
+  <si>
+    <t>P05</t>
+  </si>
+  <si>
+    <t>esito</t>
+  </si>
+  <si>
+    <t>P06</t>
+  </si>
+  <si>
+    <t>P07</t>
+  </si>
+  <si>
+    <t>hospital_sec_diagnosis</t>
   </si>
 </sst>
 </file>
@@ -372,15 +396,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,8 +423,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -413,8 +443,11 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -427,8 +460,125 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>250</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>205</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>600</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>250</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>